<commit_message>
cierre 9 Jun 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
+++ b/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>FUMIGACIONES DE   RUBEN VEGA MURAD</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>330---------334</t>
+  </si>
+  <si>
+    <t>JUNIO.,2022</t>
   </si>
 </sst>
 </file>
@@ -237,7 +240,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,6 +301,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -610,7 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -773,6 +794,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="18" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="13" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,6 +835,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC9900"/>
+      <color rgb="FFCC99FF"/>
+      <color rgb="FFCCFF99"/>
       <color rgb="FF66CCFF"/>
       <color rgb="FF0000FF"/>
       <color rgb="FF0066FF"/>
@@ -1136,7 +1174,7 @@
   <dimension ref="A2:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1157,22 +1195,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="69"/>
-      <c r="F3" s="70"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="78"/>
       <c r="G3" s="38"/>
     </row>
     <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1423,15 +1461,25 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="35"/>
+      <c r="A11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="11">
+        <v>986</v>
+      </c>
+      <c r="C11" s="35">
+        <v>346</v>
+      </c>
       <c r="D11" s="16"/>
       <c r="E11" s="35"/>
       <c r="F11" s="15"/>
       <c r="G11" s="42"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="46"/>
+      <c r="H11" s="13">
+        <v>1856</v>
+      </c>
+      <c r="I11" s="46">
+        <v>347</v>
+      </c>
       <c r="J11" s="27"/>
       <c r="K11" s="48"/>
       <c r="L11" s="13"/>
@@ -1603,100 +1651,139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K31"/>
+  <dimension ref="B3:Q31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="56" customWidth="1"/>
-    <col min="9" max="9" width="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" style="25" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="56" customWidth="1"/>
+    <col min="15" max="15" width="36" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" style="25" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B3" s="72" t="s">
+    <row r="3" spans="2:17" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B3" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="I3" s="72" t="s">
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="68"/>
+      <c r="H3" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K4" s="56"/>
-    </row>
-    <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B5" s="73" t="s">
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="O3" s="80" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E4" s="56"/>
+      <c r="Q4" s="56"/>
+    </row>
+    <row r="5" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="B5" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="73">
+        <v>44747</v>
+      </c>
+      <c r="H5" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="54" t="s">
+      <c r="I5" s="81"/>
+      <c r="J5" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="60">
+      <c r="K5" s="60">
         <v>44686</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="O5" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="64" t="s">
+      <c r="P5" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="60">
+      <c r="Q5" s="60">
         <v>44714</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="55"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="62"/>
-    </row>
-    <row r="7" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B7" s="53" t="s">
+    <row r="6" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="62"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="55"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="62"/>
+    </row>
+    <row r="7" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="B7" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="70"/>
+      <c r="D7" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="60">
+        <v>44748</v>
+      </c>
+      <c r="H7" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53" t="s">
+      <c r="I7" s="53"/>
+      <c r="J7" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="58">
+      <c r="K7" s="58">
         <v>44691</v>
       </c>
-      <c r="F7" s="63"/>
-      <c r="I7" s="53" t="s">
+      <c r="L7" s="63"/>
+      <c r="O7" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="66" t="s">
+      <c r="P7" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="58">
+      <c r="Q7" s="58">
         <v>44719</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="55"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="62"/>
-    </row>
-    <row r="9" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="62"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="55"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="62"/>
+    </row>
+    <row r="9" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B9" s="53" t="s">
         <v>26</v>
       </c>
@@ -1704,222 +1791,279 @@
       <c r="D9" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="60">
+      <c r="E9" s="58">
+        <v>44749</v>
+      </c>
+      <c r="H9" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="60">
         <v>44693</v>
       </c>
-      <c r="I9" s="53" t="s">
+      <c r="O9" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="66" t="s">
+      <c r="P9" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="60">
+      <c r="Q9" s="60">
         <v>44721</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="55"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="62"/>
-    </row>
-    <row r="11" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="62"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="55"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="62"/>
+    </row>
+    <row r="11" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B11" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="59">
+        <v>44751</v>
+      </c>
+      <c r="H11" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="53" t="s">
+      <c r="I11" s="61"/>
+      <c r="J11" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="58">
+      <c r="K11" s="58">
         <v>44695</v>
       </c>
-      <c r="I11" s="53" t="s">
+      <c r="O11" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="66" t="s">
+      <c r="P11" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="59">
+      <c r="Q11" s="59">
         <v>44723</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="55"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="62"/>
-    </row>
-    <row r="13" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="62"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="55"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="62"/>
+    </row>
+    <row r="13" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="53" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" s="53"/>
       <c r="D13" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="74">
+        <v>44756</v>
+      </c>
+      <c r="H13" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="59">
+      <c r="K13" s="59">
         <v>44695</v>
       </c>
-      <c r="I13" s="53" t="s">
+      <c r="O13" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="66" t="s">
+      <c r="P13" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="60">
+      <c r="Q13" s="60">
         <v>44728</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="55"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="62"/>
-    </row>
-    <row r="15" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="62"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="55"/>
+      <c r="O14" s="61"/>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="62"/>
+    </row>
+    <row r="15" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B15" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="61"/>
+      <c r="D15" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="75">
+        <v>44758</v>
+      </c>
+      <c r="H15" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53" t="s">
+      <c r="I15" s="53"/>
+      <c r="J15" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="60">
+      <c r="K15" s="60">
         <v>44700</v>
       </c>
-      <c r="I15" s="53" t="s">
+      <c r="O15" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="66" t="s">
+      <c r="P15" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="K15" s="58">
+      <c r="Q15" s="58">
         <v>44730</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B16" s="53"/>
       <c r="C16" s="53"/>
       <c r="D16" s="53"/>
       <c r="E16" s="55"/>
+      <c r="H16" s="53"/>
       <c r="I16" s="53"/>
-      <c r="J16" s="66"/>
+      <c r="J16" s="53"/>
       <c r="K16" s="55"/>
-    </row>
-    <row r="17" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="62"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="55"/>
-    </row>
-    <row r="18" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="55"/>
+      <c r="O16" s="53"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="55"/>
+    </row>
+    <row r="17" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="62"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="66"/>
+      <c r="Q17" s="55"/>
+    </row>
+    <row r="18" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H18" s="53"/>
       <c r="I18" s="53"/>
-      <c r="J18" s="66"/>
+      <c r="J18" s="53"/>
       <c r="K18" s="55"/>
-    </row>
-    <row r="19" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="55"/>
-    </row>
-    <row r="20" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="55"/>
-    </row>
-    <row r="21" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B21" s="53"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="55"/>
-    </row>
-    <row r="22" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="55"/>
-    </row>
-    <row r="23" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="55"/>
-    </row>
-    <row r="24" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="55"/>
-    </row>
-    <row r="25" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="55"/>
-    </row>
-    <row r="26" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="55"/>
-    </row>
-    <row r="27" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="55"/>
-    </row>
-    <row r="28" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="55"/>
-    </row>
-    <row r="29" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="55"/>
-    </row>
-    <row r="30" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="55"/>
-    </row>
-    <row r="31" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="55"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="55"/>
+    </row>
+    <row r="19" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="55"/>
+    </row>
+    <row r="20" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="55"/>
+    </row>
+    <row r="21" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="55"/>
+    </row>
+    <row r="22" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="55"/>
+    </row>
+    <row r="23" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="55"/>
+    </row>
+    <row r="24" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="55"/>
+    </row>
+    <row r="25" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="55"/>
+    </row>
+    <row r="26" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="55"/>
+    </row>
+    <row r="27" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="55"/>
+    </row>
+    <row r="28" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="55"/>
+    </row>
+    <row r="29" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="55"/>
+    </row>
+    <row r="30" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="55"/>
+    </row>
+    <row r="31" spans="8:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="55"/>
     </row>
   </sheetData>
-  <sortState ref="I5:K15">
-    <sortCondition ref="K5:K15"/>
+  <sortState ref="B5:E15">
+    <sortCondition ref="E5:E15"/>
   </sortState>
-  <mergeCells count="3">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="I3:K3"/>
+  <mergeCells count="4">
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CIERRE 19 JUL 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
+++ b/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
@@ -1177,7 +1177,7 @@
   <dimension ref="A2:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1532,8 +1532,12 @@
       <c r="I12" s="46">
         <v>364</v>
       </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="48"/>
+      <c r="J12" s="27">
+        <v>1392</v>
+      </c>
+      <c r="K12" s="48">
+        <v>375</v>
+      </c>
       <c r="L12" s="13">
         <v>1392</v>
       </c>

</xml_diff>

<commit_message>
CIERRE 12 sEPT 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
+++ b/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="35">
   <si>
     <t>FUMIGACIONES DE   RUBEN VEGA MURAD</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>4;00PM</t>
+  </si>
+  <si>
+    <t>Sept., 2022</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1214,7 @@
   <dimension ref="A2:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1621,19 +1624,45 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="51"/>
+      <c r="A14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="11">
+        <v>986</v>
+      </c>
+      <c r="C14" s="35">
+        <v>410</v>
+      </c>
+      <c r="D14" s="16">
+        <v>1392</v>
+      </c>
+      <c r="E14" s="35">
+        <v>415</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1856</v>
+      </c>
+      <c r="G14" s="42">
+        <v>414</v>
+      </c>
+      <c r="H14" s="13">
+        <v>1856</v>
+      </c>
+      <c r="I14" s="46">
+        <v>411</v>
+      </c>
+      <c r="J14" s="27">
+        <v>1392</v>
+      </c>
+      <c r="K14" s="48">
+        <v>416</v>
+      </c>
+      <c r="L14" s="13">
+        <v>1392</v>
+      </c>
+      <c r="M14" s="51">
+        <v>413</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>

</xml_diff>

<commit_message>
cierre   4 SEPT  23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
+++ b/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="64">
   <si>
     <t>FUMIGACIONES DE   RUBEN VEGA MURAD</t>
   </si>
@@ -1467,6 +1467,24 @@
     <xf numFmtId="44" fontId="9" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="14" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="14" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1500,38 +1518,20 @@
     <xf numFmtId="44" fontId="15" fillId="11" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="14" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="14" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1895,11 +1895,11 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B5" s="186" t="s">
+      <c r="B5" s="192" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="186"/>
-      <c r="D5" s="186"/>
+      <c r="C5" s="192"/>
+      <c r="D5" s="192"/>
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -2090,22 +2090,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="187" t="s">
+      <c r="C2" s="193" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="187"/>
-      <c r="E2" s="187"/>
-      <c r="F2" s="187"/>
-      <c r="G2" s="187"/>
-      <c r="H2" s="187"/>
-      <c r="I2" s="187"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
     </row>
     <row r="3" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D3" s="188" t="s">
+      <c r="D3" s="194" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="190"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="196"/>
       <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2779,7 +2779,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2804,48 +2804,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="187" t="s">
+      <c r="C2" s="193" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="187"/>
-      <c r="E2" s="187"/>
-      <c r="F2" s="187"/>
-      <c r="G2" s="187"/>
-      <c r="H2" s="187"/>
-      <c r="I2" s="187"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
     </row>
     <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D3" s="188" t="s">
+      <c r="D3" s="194" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="190"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="196"/>
       <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:18" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="191" t="s">
+      <c r="B4" s="197" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="191"/>
-      <c r="D4" s="191"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="191"/>
-      <c r="G4" s="191"/>
-      <c r="H4" s="192" t="s">
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="198" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="193"/>
-      <c r="J4" s="193"/>
-      <c r="K4" s="193"/>
-      <c r="L4" s="193"/>
-      <c r="M4" s="194"/>
+      <c r="I4" s="199"/>
+      <c r="J4" s="199"/>
+      <c r="K4" s="199"/>
+      <c r="L4" s="199"/>
+      <c r="M4" s="200"/>
       <c r="N4" s="136"/>
       <c r="O4" s="136"/>
       <c r="P4" s="136"/>
-      <c r="Q4" s="195" t="s">
+      <c r="Q4" s="201" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="196"/>
+      <c r="R4" s="202"/>
     </row>
     <row r="5" spans="1:18" s="1" customFormat="1" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
@@ -3774,17 +3774,17 @@
       </c>
     </row>
     <row r="25" spans="1:18" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="202">
+      <c r="A25" s="186">
         <v>45159</v>
       </c>
-      <c r="B25" s="203"/>
-      <c r="C25" s="204" t="s">
+      <c r="B25" s="187"/>
+      <c r="C25" s="188" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="205"/>
-      <c r="E25" s="206"/>
-      <c r="F25" s="205"/>
-      <c r="G25" s="207"/>
+      <c r="D25" s="189"/>
+      <c r="E25" s="190"/>
+      <c r="F25" s="189"/>
+      <c r="G25" s="191"/>
       <c r="H25" s="20"/>
       <c r="I25" s="37"/>
       <c r="J25" s="20"/>
@@ -3798,17 +3798,27 @@
       <c r="R25" s="42"/>
     </row>
     <row r="26" spans="1:18" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
+      <c r="A26" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="B26" s="7"/>
       <c r="C26" s="37"/>
       <c r="D26" s="9"/>
       <c r="E26" s="82"/>
       <c r="F26" s="9"/>
       <c r="G26" s="33"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="39"/>
+      <c r="H26" s="20">
+        <v>1856</v>
+      </c>
+      <c r="I26" s="37">
+        <v>803</v>
+      </c>
+      <c r="J26" s="20">
+        <v>1392</v>
+      </c>
+      <c r="K26" s="39">
+        <v>806</v>
+      </c>
       <c r="L26" s="184"/>
       <c r="M26" s="127"/>
       <c r="N26" s="184"/>
@@ -4146,48 +4156,48 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:102" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="BK3" s="186" t="s">
+      <c r="BK3" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="BL3" s="186"/>
-      <c r="BM3" s="186"/>
+      <c r="BL3" s="192"/>
+      <c r="BM3" s="192"/>
       <c r="BN3" s="60"/>
-      <c r="BQ3" s="186" t="s">
+      <c r="BQ3" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="BR3" s="186"/>
-      <c r="BS3" s="186"/>
+      <c r="BR3" s="192"/>
+      <c r="BS3" s="192"/>
       <c r="BT3" s="60"/>
-      <c r="BW3" s="186" t="s">
+      <c r="BW3" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="BX3" s="186"/>
-      <c r="BY3" s="186"/>
+      <c r="BX3" s="192"/>
+      <c r="BY3" s="192"/>
       <c r="BZ3" s="60"/>
-      <c r="CB3" s="186" t="s">
+      <c r="CB3" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="CC3" s="186"/>
-      <c r="CD3" s="186"/>
+      <c r="CC3" s="192"/>
+      <c r="CD3" s="192"/>
       <c r="CE3" s="60"/>
-      <c r="CI3" s="186" t="s">
+      <c r="CI3" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="CJ3" s="186"/>
-      <c r="CK3" s="186"/>
+      <c r="CJ3" s="192"/>
+      <c r="CK3" s="192"/>
       <c r="CL3" s="60"/>
       <c r="CM3" s="59"/>
-      <c r="CO3" s="186" t="s">
+      <c r="CO3" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="CP3" s="186"/>
-      <c r="CQ3" s="186"/>
-      <c r="CR3" s="186"/>
-      <c r="CV3" s="186" t="s">
+      <c r="CP3" s="192"/>
+      <c r="CQ3" s="192"/>
+      <c r="CR3" s="192"/>
+      <c r="CV3" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="CW3" s="186"/>
-      <c r="CX3" s="186"/>
+      <c r="CW3" s="192"/>
+      <c r="CX3" s="192"/>
     </row>
     <row r="4" spans="2:102" x14ac:dyDescent="0.25">
       <c r="B4" s="144"/>
@@ -4202,66 +4212,66 @@
       <c r="CX4" s="47"/>
     </row>
     <row r="5" spans="2:102" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B5" s="197" t="s">
+      <c r="B5" s="204" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="198"/>
-      <c r="D5" s="198"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="205"/>
       <c r="E5" s="148"/>
-      <c r="H5" s="186" t="s">
+      <c r="H5" s="192" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="186"/>
-      <c r="J5" s="186"/>
+      <c r="I5" s="192"/>
+      <c r="J5" s="192"/>
       <c r="K5" s="60"/>
-      <c r="O5" s="186" t="s">
+      <c r="O5" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="186"/>
-      <c r="Q5" s="186"/>
+      <c r="P5" s="192"/>
+      <c r="Q5" s="192"/>
       <c r="R5" s="60"/>
-      <c r="U5" s="186" t="s">
+      <c r="U5" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="V5" s="186"/>
-      <c r="W5" s="186"/>
+      <c r="V5" s="192"/>
+      <c r="W5" s="192"/>
       <c r="X5" s="60"/>
-      <c r="AA5" s="186" t="s">
+      <c r="AA5" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="AB5" s="186"/>
-      <c r="AC5" s="186"/>
+      <c r="AB5" s="192"/>
+      <c r="AC5" s="192"/>
       <c r="AD5" s="60"/>
       <c r="AE5" s="85"/>
-      <c r="AG5" s="186" t="s">
+      <c r="AG5" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="AH5" s="186"/>
-      <c r="AI5" s="186"/>
+      <c r="AH5" s="192"/>
+      <c r="AI5" s="192"/>
       <c r="AJ5" s="60"/>
-      <c r="AN5" s="186" t="s">
+      <c r="AN5" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="AO5" s="186"/>
-      <c r="AP5" s="186"/>
+      <c r="AO5" s="192"/>
+      <c r="AP5" s="192"/>
       <c r="AQ5" s="60"/>
-      <c r="AS5" s="186" t="s">
+      <c r="AS5" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="AT5" s="186"/>
-      <c r="AU5" s="186"/>
+      <c r="AT5" s="192"/>
+      <c r="AU5" s="192"/>
       <c r="AV5" s="60"/>
-      <c r="AY5" s="186" t="s">
+      <c r="AY5" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="AZ5" s="186"/>
-      <c r="BA5" s="186"/>
+      <c r="AZ5" s="192"/>
+      <c r="BA5" s="192"/>
       <c r="BB5" s="60"/>
-      <c r="BE5" s="186" t="s">
+      <c r="BE5" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="BF5" s="186"/>
-      <c r="BG5" s="186"/>
+      <c r="BF5" s="192"/>
+      <c r="BG5" s="192"/>
       <c r="BH5" s="60"/>
       <c r="BK5" s="61" t="s">
         <v>23</v>
@@ -4313,10 +4323,10 @@
       <c r="CL5" s="51">
         <v>44747</v>
       </c>
-      <c r="CO5" s="201" t="s">
+      <c r="CO5" s="203" t="s">
         <v>23</v>
       </c>
-      <c r="CP5" s="201"/>
+      <c r="CP5" s="203"/>
       <c r="CQ5" s="45" t="s">
         <v>15</v>
       </c>
@@ -4334,11 +4344,11 @@
       </c>
     </row>
     <row r="6" spans="2:102" ht="21" x14ac:dyDescent="0.35">
-      <c r="B6" s="199" t="s">
+      <c r="B6" s="206" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="200"/>
-      <c r="D6" s="200"/>
+      <c r="C6" s="207"/>
+      <c r="D6" s="207"/>
       <c r="E6" s="149"/>
       <c r="K6" s="47"/>
       <c r="R6" s="47"/>
@@ -5842,6 +5852,18 @@
     <sortCondition ref="E8:E21"/>
   </sortState>
   <mergeCells count="19">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="CO5:CP5"/>
+    <mergeCell ref="BE5:BG5"/>
+    <mergeCell ref="AA5:AC5"/>
+    <mergeCell ref="AG5:AI5"/>
+    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="AS5:AU5"/>
+    <mergeCell ref="AY5:BA5"/>
     <mergeCell ref="CV3:CX3"/>
     <mergeCell ref="CI3:CK3"/>
     <mergeCell ref="CB3:CD3"/>
@@ -5849,18 +5871,6 @@
     <mergeCell ref="BQ3:BS3"/>
     <mergeCell ref="BW3:BY3"/>
     <mergeCell ref="CO3:CR3"/>
-    <mergeCell ref="CO5:CP5"/>
-    <mergeCell ref="BE5:BG5"/>
-    <mergeCell ref="AA5:AC5"/>
-    <mergeCell ref="AG5:AI5"/>
-    <mergeCell ref="AN5:AP5"/>
-    <mergeCell ref="AS5:AU5"/>
-    <mergeCell ref="AY5:BA5"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="U5:W5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CIERRE 24 OCT 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
+++ b/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
@@ -4206,7 +4206,7 @@
   <dimension ref="B3:DL31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4967,7 +4967,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="163">
-        <v>45236</v>
+        <v>45238</v>
       </c>
       <c r="J10" s="162" t="s">
         <v>21</v>
@@ -5220,7 +5220,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="166">
-        <v>45237</v>
+        <v>45240</v>
       </c>
       <c r="J12" s="153" t="s">
         <v>19</v>
@@ -6252,13 +6252,6 @@
     <sortCondition ref="S8:S21"/>
   </sortState>
   <mergeCells count="23">
-    <mergeCell ref="BG5:BI5"/>
-    <mergeCell ref="BM5:BO5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="AC5:AE5"/>
-    <mergeCell ref="AI5:AK5"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="J5:L5"/>
@@ -6275,6 +6268,13 @@
     <mergeCell ref="AO5:AQ5"/>
     <mergeCell ref="AU5:AW5"/>
     <mergeCell ref="BB5:BD5"/>
+    <mergeCell ref="BG5:BI5"/>
+    <mergeCell ref="BM5:BO5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="AC5:AE5"/>
+    <mergeCell ref="AI5:AK5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 13 ENE 24
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
+++ b/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="87">
   <si>
     <t>FUMIGACIONES DE   RUBEN VEGA MURAD</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>8-ENE--24</t>
+  </si>
+  <si>
+    <t>8-Ene-,23</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="236">
+  <cellXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1668,20 +1671,23 @@
     <xf numFmtId="44" fontId="15" fillId="11" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="44" fontId="5" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1692,6 +1698,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC99FF"/>
       <color rgb="FF0000FF"/>
       <color rgb="FF00FF00"/>
       <color rgb="FF66FFFF"/>
@@ -1700,7 +1707,6 @@
       <color rgb="FFFFCCFF"/>
       <color rgb="FFFF66FF"/>
       <color rgb="FF66CCFF"/>
-      <color rgb="FFCC99FF"/>
       <color rgb="FF0066FF"/>
     </mruColors>
   </colors>
@@ -2927,9 +2933,9 @@
   </sheetPr>
   <dimension ref="A2:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L34" sqref="L34"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3044,7 +3050,7 @@
         <v>5</v>
       </c>
       <c r="P5" s="137"/>
-      <c r="Q5" s="90" t="s">
+      <c r="Q5" s="236" t="s">
         <v>59</v>
       </c>
       <c r="R5" s="25" t="s">
@@ -4291,8 +4297,12 @@
       <c r="A33" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="37"/>
+      <c r="B33" s="7">
+        <v>986</v>
+      </c>
+      <c r="C33" s="37">
+        <v>997</v>
+      </c>
       <c r="D33" s="9">
         <v>1392</v>
       </c>
@@ -4343,8 +4353,12 @@
       <c r="I34" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="J34" s="20"/>
-      <c r="K34" s="39"/>
+      <c r="J34" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="K34" s="39" t="s">
+        <v>80</v>
+      </c>
       <c r="L34" s="184"/>
       <c r="M34" s="127"/>
       <c r="N34" s="184"/>
@@ -4623,35 +4637,35 @@
       <c r="EB4" s="47"/>
     </row>
     <row r="5" spans="2:132" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B5" s="232" t="s">
+      <c r="B5" s="231" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="233"/>
-      <c r="D5" s="233"/>
+      <c r="C5" s="232"/>
+      <c r="D5" s="232"/>
       <c r="E5" s="148"/>
-      <c r="J5" s="232" t="s">
+      <c r="J5" s="231" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="233"/>
-      <c r="L5" s="233"/>
+      <c r="K5" s="232"/>
+      <c r="L5" s="232"/>
       <c r="M5" s="148"/>
-      <c r="R5" s="232" t="s">
+      <c r="R5" s="231" t="s">
         <v>55</v>
       </c>
-      <c r="S5" s="233"/>
-      <c r="T5" s="233"/>
+      <c r="S5" s="232"/>
+      <c r="T5" s="232"/>
       <c r="U5" s="148"/>
-      <c r="Z5" s="232" t="s">
+      <c r="Z5" s="231" t="s">
         <v>55</v>
       </c>
-      <c r="AA5" s="233"/>
-      <c r="AB5" s="233"/>
+      <c r="AA5" s="232"/>
+      <c r="AB5" s="232"/>
       <c r="AC5" s="148"/>
-      <c r="AF5" s="232" t="s">
+      <c r="AF5" s="231" t="s">
         <v>55</v>
       </c>
-      <c r="AG5" s="233"/>
-      <c r="AH5" s="233"/>
+      <c r="AG5" s="232"/>
+      <c r="AH5" s="232"/>
       <c r="AI5" s="148"/>
       <c r="AL5" s="220" t="s">
         <v>55</v>
@@ -4758,10 +4772,10 @@
       <c r="DP5" s="51">
         <v>44747</v>
       </c>
-      <c r="DS5" s="231" t="s">
+      <c r="DS5" s="235" t="s">
         <v>23</v>
       </c>
-      <c r="DT5" s="231"/>
+      <c r="DT5" s="235"/>
       <c r="DU5" s="45" t="s">
         <v>15</v>
       </c>
@@ -4779,35 +4793,35 @@
       </c>
     </row>
     <row r="6" spans="2:132" ht="21" x14ac:dyDescent="0.35">
-      <c r="B6" s="234" t="s">
+      <c r="B6" s="233" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="235"/>
-      <c r="D6" s="235"/>
+      <c r="C6" s="234"/>
+      <c r="D6" s="234"/>
       <c r="E6" s="149"/>
-      <c r="J6" s="234" t="s">
+      <c r="J6" s="233" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="235"/>
-      <c r="L6" s="235"/>
+      <c r="K6" s="234"/>
+      <c r="L6" s="234"/>
       <c r="M6" s="149"/>
-      <c r="R6" s="234" t="s">
+      <c r="R6" s="233" t="s">
         <v>62</v>
       </c>
-      <c r="S6" s="235"/>
-      <c r="T6" s="235"/>
+      <c r="S6" s="234"/>
+      <c r="T6" s="234"/>
       <c r="U6" s="149"/>
-      <c r="Z6" s="234" t="s">
+      <c r="Z6" s="233" t="s">
         <v>62</v>
       </c>
-      <c r="AA6" s="235"/>
-      <c r="AB6" s="235"/>
+      <c r="AA6" s="234"/>
+      <c r="AB6" s="234"/>
       <c r="AC6" s="149"/>
-      <c r="AF6" s="234" t="s">
+      <c r="AF6" s="233" t="s">
         <v>62</v>
       </c>
-      <c r="AG6" s="235"/>
-      <c r="AH6" s="235"/>
+      <c r="AG6" s="234"/>
+      <c r="AH6" s="234"/>
       <c r="AI6" s="149"/>
       <c r="AO6" s="47"/>
       <c r="AV6" s="47"/>
@@ -6792,6 +6806,19 @@
     <sortCondition ref="E8:E22"/>
   </sortState>
   <mergeCells count="27">
+    <mergeCell ref="DS5:DT5"/>
+    <mergeCell ref="CI5:CK5"/>
+    <mergeCell ref="BE5:BG5"/>
+    <mergeCell ref="BK5:BM5"/>
+    <mergeCell ref="BR5:BT5"/>
+    <mergeCell ref="CC5:CE5"/>
+    <mergeCell ref="DZ3:EB3"/>
+    <mergeCell ref="DM3:DO3"/>
+    <mergeCell ref="DF3:DH3"/>
+    <mergeCell ref="CO3:CQ3"/>
+    <mergeCell ref="CU3:CW3"/>
+    <mergeCell ref="DA3:DC3"/>
+    <mergeCell ref="DS3:DV3"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="J5:L5"/>
@@ -6806,19 +6833,6 @@
     <mergeCell ref="AL5:AN5"/>
     <mergeCell ref="AS5:AU5"/>
     <mergeCell ref="AY5:BA5"/>
-    <mergeCell ref="DZ3:EB3"/>
-    <mergeCell ref="DM3:DO3"/>
-    <mergeCell ref="DF3:DH3"/>
-    <mergeCell ref="CO3:CQ3"/>
-    <mergeCell ref="CU3:CW3"/>
-    <mergeCell ref="DA3:DC3"/>
-    <mergeCell ref="DS3:DV3"/>
-    <mergeCell ref="DS5:DT5"/>
-    <mergeCell ref="CI5:CK5"/>
-    <mergeCell ref="BE5:BG5"/>
-    <mergeCell ref="BK5:BM5"/>
-    <mergeCell ref="BR5:BT5"/>
-    <mergeCell ref="CC5:CE5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
cierre 18 ene 24
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
+++ b/01 DOCUEMENTOS/FUMIFACION RUBEN  2022.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="92">
   <si>
     <t>FUMIGACIONES DE   RUBEN VEGA MURAD</t>
   </si>
@@ -1140,7 +1140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="239">
+  <cellXfs count="240">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1711,19 +1711,22 @@
     <xf numFmtId="44" fontId="15" fillId="11" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2970,9 +2973,9 @@
   </sheetPr>
   <dimension ref="A2:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4373,8 +4376,12 @@
         <v>999</v>
       </c>
       <c r="P33" s="138"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="42"/>
+      <c r="Q33" s="9">
+        <v>1392</v>
+      </c>
+      <c r="R33" s="42">
+        <v>1002</v>
+      </c>
     </row>
     <row r="34" spans="1:18" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="5"/>
@@ -4417,8 +4424,12 @@
         <v>80</v>
       </c>
       <c r="P34" s="138"/>
-      <c r="Q34" s="9"/>
-      <c r="R34" s="42"/>
+      <c r="Q34" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="R34" s="239" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="35" spans="1:18" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
@@ -4690,35 +4701,35 @@
       <c r="EB4" s="47"/>
     </row>
     <row r="5" spans="2:132" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B5" s="235" t="s">
+      <c r="B5" s="234" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="236"/>
-      <c r="D5" s="236"/>
+      <c r="C5" s="235"/>
+      <c r="D5" s="235"/>
       <c r="E5" s="148"/>
-      <c r="J5" s="235" t="s">
+      <c r="J5" s="234" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="236"/>
-      <c r="L5" s="236"/>
+      <c r="K5" s="235"/>
+      <c r="L5" s="235"/>
       <c r="M5" s="148"/>
-      <c r="R5" s="235" t="s">
+      <c r="R5" s="234" t="s">
         <v>55</v>
       </c>
-      <c r="S5" s="236"/>
-      <c r="T5" s="236"/>
+      <c r="S5" s="235"/>
+      <c r="T5" s="235"/>
       <c r="U5" s="148"/>
-      <c r="Z5" s="235" t="s">
+      <c r="Z5" s="234" t="s">
         <v>55</v>
       </c>
-      <c r="AA5" s="236"/>
-      <c r="AB5" s="236"/>
+      <c r="AA5" s="235"/>
+      <c r="AB5" s="235"/>
       <c r="AC5" s="148"/>
-      <c r="AF5" s="235" t="s">
+      <c r="AF5" s="234" t="s">
         <v>55</v>
       </c>
-      <c r="AG5" s="236"/>
-      <c r="AH5" s="236"/>
+      <c r="AG5" s="235"/>
+      <c r="AH5" s="235"/>
       <c r="AI5" s="148"/>
       <c r="AL5" s="223" t="s">
         <v>55</v>
@@ -4825,10 +4836,10 @@
       <c r="DP5" s="51">
         <v>44747</v>
       </c>
-      <c r="DS5" s="234" t="s">
+      <c r="DS5" s="238" t="s">
         <v>23</v>
       </c>
-      <c r="DT5" s="234"/>
+      <c r="DT5" s="238"/>
       <c r="DU5" s="45" t="s">
         <v>15</v>
       </c>
@@ -4846,35 +4857,35 @@
       </c>
     </row>
     <row r="6" spans="2:132" ht="21" x14ac:dyDescent="0.35">
-      <c r="B6" s="237" t="s">
+      <c r="B6" s="236" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="238"/>
-      <c r="D6" s="238"/>
+      <c r="C6" s="237"/>
+      <c r="D6" s="237"/>
       <c r="E6" s="149"/>
-      <c r="J6" s="237" t="s">
+      <c r="J6" s="236" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="238"/>
-      <c r="L6" s="238"/>
+      <c r="K6" s="237"/>
+      <c r="L6" s="237"/>
       <c r="M6" s="149"/>
-      <c r="R6" s="237" t="s">
+      <c r="R6" s="236" t="s">
         <v>62</v>
       </c>
-      <c r="S6" s="238"/>
-      <c r="T6" s="238"/>
+      <c r="S6" s="237"/>
+      <c r="T6" s="237"/>
       <c r="U6" s="149"/>
-      <c r="Z6" s="237" t="s">
+      <c r="Z6" s="236" t="s">
         <v>62</v>
       </c>
-      <c r="AA6" s="238"/>
-      <c r="AB6" s="238"/>
+      <c r="AA6" s="237"/>
+      <c r="AB6" s="237"/>
       <c r="AC6" s="149"/>
-      <c r="AF6" s="237" t="s">
+      <c r="AF6" s="236" t="s">
         <v>62</v>
       </c>
-      <c r="AG6" s="238"/>
-      <c r="AH6" s="238"/>
+      <c r="AG6" s="237"/>
+      <c r="AH6" s="237"/>
       <c r="AI6" s="149"/>
       <c r="AO6" s="47"/>
       <c r="AV6" s="47"/>
@@ -6859,6 +6870,19 @@
     <sortCondition ref="E8:E22"/>
   </sortState>
   <mergeCells count="27">
+    <mergeCell ref="DS5:DT5"/>
+    <mergeCell ref="CI5:CK5"/>
+    <mergeCell ref="BE5:BG5"/>
+    <mergeCell ref="BK5:BM5"/>
+    <mergeCell ref="BR5:BT5"/>
+    <mergeCell ref="CC5:CE5"/>
+    <mergeCell ref="DZ3:EB3"/>
+    <mergeCell ref="DM3:DO3"/>
+    <mergeCell ref="DF3:DH3"/>
+    <mergeCell ref="CO3:CQ3"/>
+    <mergeCell ref="CU3:CW3"/>
+    <mergeCell ref="DA3:DC3"/>
+    <mergeCell ref="DS3:DV3"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="J5:L5"/>
@@ -6873,19 +6897,6 @@
     <mergeCell ref="AL5:AN5"/>
     <mergeCell ref="AS5:AU5"/>
     <mergeCell ref="AY5:BA5"/>
-    <mergeCell ref="DZ3:EB3"/>
-    <mergeCell ref="DM3:DO3"/>
-    <mergeCell ref="DF3:DH3"/>
-    <mergeCell ref="CO3:CQ3"/>
-    <mergeCell ref="CU3:CW3"/>
-    <mergeCell ref="DA3:DC3"/>
-    <mergeCell ref="DS3:DV3"/>
-    <mergeCell ref="DS5:DT5"/>
-    <mergeCell ref="CI5:CK5"/>
-    <mergeCell ref="BE5:BG5"/>
-    <mergeCell ref="BK5:BM5"/>
-    <mergeCell ref="BR5:BT5"/>
-    <mergeCell ref="CC5:CE5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>